<commit_message>
Anrede und PATIENT in Lua
</commit_message>
<xml_diff>
--- a/Praxis1.xlsx
+++ b/Praxis1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">Frau</t>
   </si>
   <si>
-    <t xml:space="preserve">Alpa</t>
+    <t xml:space="preserve">Alpha</t>
   </si>
   <si>
     <t xml:space="preserve">Alphason</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">Astraße 1</t>
   </si>
   <si>
-    <t xml:space="preserve">12345 UÜ üü</t>
+    <t xml:space="preserve">ÄäÜüÖößstadt</t>
   </si>
   <si>
     <t xml:space="preserve">Herrn Dr. Foo</t>
@@ -161,9 +161,6 @@
     <t xml:space="preserve">Bstraße 2</t>
   </si>
   <si>
-    <t xml:space="preserve">23456 OÖ öö</t>
-  </si>
-  <si>
     <t xml:space="preserve">Herrn Bar</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cstraße 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34567 AÄ ää</t>
   </si>
 </sst>
 </file>
@@ -553,7 +547,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="1" sqref="G4 D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -973,7 +967,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1073,17 +1067,17 @@
       <c r="F3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>44510</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,19 +1088,19 @@
         <v>37228</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>52</v>
+      <c r="G4" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="19"/>

</xml_diff>

<commit_message>
Einleitung in Lua, escape in Python
</commit_message>
<xml_diff>
--- a/Praxis1.xlsx
+++ b/Praxis1.xlsx
@@ -146,7 +146,7 @@
     <t xml:space="preserve">Herrn Dr. Foo</t>
   </si>
   <si>
-    <t xml:space="preserve">aaa bbb ccc aaa bbb ccc aaa bbb ccc aaa bbb ccc aaa bbb ccc aaa bbb ccc aaa bbb ccc</t>
+    <t xml:space="preserve">aaa bbb ccc  &amp; % $ # _ { } ~ ^ \  / ( ) = ? § ! “ aaa “bbb” ccc aaa bbb ccc aaa bbb ccc aaa bbb ccc aaa bbb ccc aaa bbb ccc &amp; so weiter</t>
   </si>
   <si>
     <t xml:space="preserve">Herr</t>
@@ -547,7 +547,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D17" activeCellId="1" sqref="G4 D17"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -964,10 +964,10 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Test "Skipping invoice {} because it has no date"
</commit_message>
<xml_diff>
--- a/Praxis1.xlsx
+++ b/Praxis1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Behandlungen" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -101,6 +101,12 @@
     <t xml:space="preserve">2022-003</t>
   </si>
   <si>
+    <t xml:space="preserve">Nix Nixus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-004</t>
+  </si>
+  <si>
     <t xml:space="preserve">Datum Rechnung</t>
   </si>
   <si>
@@ -177,6 +183,15 @@
   </si>
   <si>
     <t xml:space="preserve">Cstraße 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frau Nix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nixus</t>
   </si>
 </sst>
 </file>
@@ -542,12 +557,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="N11" activeCellId="0" sqref="N11:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -939,9 +954,35 @@
         <v>35.5</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="18" t="n">
+        <v>37214</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="N11" s="6" t="n">
+        <f aca="false">SUM(F11:L11)</f>
+        <v>33</v>
+      </c>
+      <c r="O11" s="19"/>
+      <c r="P11" s="21" t="n">
+        <f aca="false">N11+M11</f>
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:P10"/>
-  <conditionalFormatting sqref="O8:O9 O1:O6 O11:O1048576">
+  <conditionalFormatting sqref="O8:O9 O1:O6 O12:O1048576">
     <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -964,10 +1005,10 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="N11:P11 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -989,31 +1030,31 @@
         <v>4</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,28 +1065,28 @@
         <v>37226</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I2" s="18" t="n">
         <v>44497</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,28 +1097,28 @@
         <v>37227</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>44510</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1088,26 +1129,36 @@
         <v>37228</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="H5" s="19"/>
       <c r="I5" s="18"/>
       <c r="J5" s="19"/>

</xml_diff>